<commit_message>
Added generation of tables and charts for second research question.
</commit_message>
<xml_diff>
--- a/result/experiments/correlation/tables.xlsx
+++ b/result/experiments/correlation/tables.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,16 @@
           <t>CaT</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>p MCI</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p CaT</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,6 +478,16 @@
           <t>0.9967198029349986</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2.890401367330267e-176</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -485,6 +505,16 @@
           <t>0.9967686348629464</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1.3413499318584676e-178</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,12 +524,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.8051755277741818</t>
+          <t>0.8052113335069778</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9968525194124408</t>
+          <t>0.9968517538954185</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1.1772177295534556e-179</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -519,6 +559,16 @@
           <t>0.9968821328340922</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6.4091617714916105e-180</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -536,6 +586,16 @@
           <t>0.9969194820067057</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4.480209739718794e-180</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,6 +611,16 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>0.9969433741958748</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3.3311560956054236e-180</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -565,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,6 +664,21 @@
           <t>ADS</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p eMCI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p CE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>p ADS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -603,17 +688,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.6598901054840083</t>
+          <t>0.6596577634481592</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9016958287883972</t>
+          <t>0.9021384111776304</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>0.9277153322571089</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.97039923112561e-14</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2.1664746371285588e-39</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
         </is>
       </c>
     </row>
@@ -625,17 +725,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.6835373615770917</t>
+          <t>0.6833179274321232</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9076886335723375</t>
+          <t>0.9081312159615705</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>0.9277153322571089</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>9.658454960015145e-16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>9.770536689820019e-41</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
         </is>
       </c>
     </row>
@@ -660,6 +775,21 @@
           <t>0.9277153322571089</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3.454151027545609e-16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5.655150367971526e-41</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -682,6 +812,21 @@
           <t>0.9277153322571089</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2.3319681813256577e-16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5.215383022435058e-41</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -704,6 +849,21 @@
           <t>0.9277153322571089</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2.1507040053039045e-16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>3.9050640248741784e-41</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -724,6 +884,21 @@
       <c r="D7" t="inlineStr">
         <is>
           <t>0.9277153322571089</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2.0971555605831855e-16</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3.035868346498158e-41</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>7.030296389889929e-46</t>
         </is>
       </c>
     </row>
@@ -738,7 +913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +942,21 @@
           <t>AIS</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p aMCI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p CA</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>p AIS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -776,17 +966,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.611594690557984</t>
+          <t>0.6114731168666006</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.8270190650583528</t>
+          <t>0.8275038020796129</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>0.8372650454873967</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4.251954503617643e-12</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1.4277782627364748e-27</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>9.246331116844667e-29</t>
         </is>
       </c>
     </row>
@@ -798,17 +1003,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.6211746974389971</t>
+          <t>0.6213813727143489</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.8374466816942742</t>
+          <t>0.8369850273883119</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.849494851069834</t>
+          <t>0.8492216567436105</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1.5179206961126375e-12</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1.002661049872069e-28</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.5017857929065715e-30</t>
         </is>
       </c>
     </row>
@@ -833,6 +1053,21 @@
           <t>0.8543949110061435</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.3045158516034313e-12</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>9.698270577594554e-30</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4.756625901484599e-31</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -855,6 +1090,21 @@
           <t>0.8549994261109788</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.2379174417710588e-12</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>7.930521101766723e-30</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3.9015553291475096e-31</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -877,6 +1127,21 @@
           <t>0.8560340769634855</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1.291091984587231e-12</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5.157354712313424e-30</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2.7735229151705236e-31</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -886,17 +1151,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.6232475288770843</t>
+          <t>0.6231137978165625</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8468644295359032</t>
+          <t>0.8473491665571636</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>0.8563072712897092</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1.263008095595311e-12</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4.493406795425381e-30</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2.5334103499330056e-31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added generation of tables for third research question.
</commit_message>
<xml_diff>
--- a/result/experiments/correlation/tables.xlsx
+++ b/result/experiments/correlation/tables.xlsx
@@ -470,17 +470,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.8007993929010384</t>
+          <t>0.8008077507378715</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9967198029349986</t>
+          <t>0.9966966762628516</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.890401367330267e-176</t>
+          <t>2.8485047010099122e-176</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -497,17 +497,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.8038481513244287</t>
+          <t>0.8038552744808205</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9967686348629464</t>
+          <t>0.9967554196217195</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.3413499318584676e-178</t>
+          <t>1.3244701182945045e-178</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -524,17 +524,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.8052113335069778</t>
+          <t>0.8051098047845403</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9968517538954185</t>
+          <t>0.9968393041712138</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.1772177295534556e-179</t>
+          <t>1.412037977879303e-179</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,17 +551,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.8055503007758079</t>
+          <t>0.8054873320733046</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9968821328340922</t>
+          <t>0.9968656137825587</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.4091617714916105e-180</t>
+          <t>7.176179319103765e-180</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -578,17 +578,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.8057496066916499</t>
+          <t>0.8056827439969856</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9969194820067057</t>
+          <t>0.9969029629551722</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4.480209739718794e-180</t>
+          <t>5.052266325892004e-180</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -605,17 +605,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.8059143890428464</t>
+          <t>0.8058475263481822</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9969433741958748</t>
+          <t>0.9969268551443414</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3.3311560956054236e-180</t>
+          <t>3.7569295251008913e-180</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -688,12 +688,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.6596577634481592</t>
+          <t>0.6588703821044485</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9021384111776304</t>
+          <t>0.9017317138469837</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -703,12 +703,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1.97039923112561e-14</t>
+          <t>2.1683142794392424e-14</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.1664746371285588e-39</t>
+          <t>2.65411609941841e-39</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -762,12 +762,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.6909077672698595</t>
+          <t>0.6910626619604255</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9091479592881873</t>
+          <t>0.9087412619575406</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -777,12 +777,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3.454151027545609e-16</t>
+          <t>3.3813124186177687e-16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5.655150367971526e-41</t>
+          <t>7.043154721392135e-41</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -799,12 +799,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.6937475032635704</t>
+          <t>0.6930504771560232</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9092974803656309</t>
+          <t>0.9088907830349844</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -814,12 +814,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2.3319681813256577e-16</t>
+          <t>2.569115925704546e-16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5.215383022435058e-41</t>
+          <t>6.497913657903211e-41</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.6943283583531931</t>
+          <t>0.6945477924981616</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9098297754013301</t>
+          <t>0.9098477179306234</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -851,12 +851,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.1507040053039045e-16</t>
+          <t>2.0858504654349297e-16</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3.9050640248741784e-41</t>
+          <t>3.867042441661209e-41</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -966,32 +966,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.6114731168666006</t>
+          <t>0.6117648937259206</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.8275038020796129</t>
+          <t>0.8273653057878243</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.8372650454873967</t>
+          <t>0.8374219869088442</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4.251954503617643e-12</t>
+          <t>4.127030022590549e-12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.4277782627364748e-27</t>
+          <t>1.4824732952094078e-27</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>9.246331116844667e-29</t>
+          <t>8.835280874051889e-29</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.6213813727143489</t>
+          <t>0.6215151037748706</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1013,12 +1013,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.8492216567436105</t>
+          <t>0.8489484624173868</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.5179206961126375e-12</t>
+          <t>1.4965916047525061e-12</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.5017857929065715e-30</t>
+          <t>2.7262781976356816e-30</t>
         </is>
       </c>
     </row>
@@ -1040,12 +1040,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.6228098635881041</t>
+          <t>0.622663975158444</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.8448504626261429</t>
+          <t>0.8445734700425658</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.3045158516034313e-12</t>
+          <t>1.3249048902810494e-12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>9.698270577594554e-30</t>
+          <t>1.055285308032373e-29</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.6229071225412108</t>
+          <t>0.6230286962325943</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.291091984587231e-12</t>
+          <t>1.2744998035215815e-12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">

</xml_diff>